<commit_message>
converter jin to kg unit
</commit_message>
<xml_diff>
--- a/excel/ingredient2018115.xlsx
+++ b/excel/ingredient2018115.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="43">
   <si>
     <t>供餐日期</t>
   </si>
@@ -83,7 +83,7 @@
     <t>新加南食品行</t>
   </si>
   <si>
-    <t>25.8斤</t>
+    <t>15.0</t>
   </si>
   <si>
     <t>Y</t>
@@ -98,7 +98,7 @@
     <t>雞肉</t>
   </si>
   <si>
-    <t>12斤</t>
+    <t>7.199999999999999</t>
   </si>
   <si>
     <t>創意炒蛋</t>
@@ -107,7 +107,7 @@
     <t>皮蛋</t>
   </si>
   <si>
-    <t>8顆</t>
+    <t>1.7999999999999998</t>
   </si>
   <si>
     <t>鹹蛋</t>
@@ -119,7 +119,7 @@
     <t>菠菜</t>
   </si>
   <si>
-    <t>8斤</t>
+    <t>4.8</t>
   </si>
   <si>
     <t>肉羹湯</t>
@@ -128,22 +128,19 @@
     <t>肉羹</t>
   </si>
   <si>
-    <t>4斤</t>
+    <t>2.4</t>
   </si>
   <si>
     <t>竹筍絲</t>
   </si>
   <si>
-    <t>1斤</t>
+    <t>0.6</t>
   </si>
   <si>
     <t>木耳</t>
   </si>
   <si>
     <t>柴魚片</t>
-  </si>
-  <si>
-    <t>1包</t>
   </si>
 </sst>
 </file>
@@ -640,7 +637,7 @@
       <c r="L10"/>
       <c r="M10"/>
       <c r="N10" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="O10" t="s">
         <v>24</v>

</xml_diff>